<commit_message>
moving to different pc
</commit_message>
<xml_diff>
--- a/Formula 1.xlsx
+++ b/Formula 1.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Youtube VD\Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\OpenLAP-Lap-Time-Simulator-Refactor\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECB22B8-D4C9-40A1-A5A2-70CA336D747E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8745" windowHeight="12405"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
     <sheet name="Torque Curve" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="139">
   <si>
     <t>General</t>
   </si>
@@ -198,9 +210,6 @@
     <t>Drive Type</t>
   </si>
   <si>
-    <t>RWD</t>
-  </si>
-  <si>
     <t>[Steering Wheel Angle]/[Wheel Angle]</t>
   </si>
   <si>
@@ -328,12 +337,129 @@
   </si>
   <si>
     <t>From crancskaft to Input shaft.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>OpenVEHICLE Name</t>
+  </si>
+  <si>
+    <t>Lapsim Name</t>
+  </si>
+  <si>
+    <t>Powertrain.Drivetype</t>
+  </si>
+  <si>
+    <t>Aero.calculateLift()</t>
+  </si>
+  <si>
+    <t>Aero.calculateDrag()</t>
+  </si>
+  <si>
+    <t>Aero.CLScaleMultiplier</t>
+  </si>
+  <si>
+    <t>Aero.CDScaleMultiplier</t>
+  </si>
+  <si>
+    <t>Aero.CentreOfPressure</t>
+  </si>
+  <si>
+    <t>Baked into aeromap</t>
+  </si>
+  <si>
+    <t>Not sure how used yet</t>
+  </si>
+  <si>
+    <t>In lapsim settings</t>
+  </si>
+  <si>
+    <t>Unnecessary?</t>
+  </si>
+  <si>
+    <t>Tyres.(Long/Lat)GripScaling</t>
+  </si>
+  <si>
+    <t>Tyres.Radius</t>
+  </si>
+  <si>
+    <t>Tyres.RollingResistance</t>
+  </si>
+  <si>
+    <t>Powertrain.Motor.PowerFactorMultiplier</t>
+  </si>
+  <si>
+    <t>Powertrain.Motor.ThermalEfficiency</t>
+  </si>
+  <si>
+    <t>Powertrain.Motor.FuelLowerHeatingValue</t>
+  </si>
+  <si>
+    <t>Powertrain.Transmission.ShiftTime</t>
+  </si>
+  <si>
+    <t>Powertrain.Transmission.PrimaryGearEfficiency</t>
+  </si>
+  <si>
+    <t>Powertrain.Transmission.FinalGearEfficiency</t>
+  </si>
+  <si>
+    <t>Powertrain.Transmission.GearboxEfficiency</t>
+  </si>
+  <si>
+    <t>Powertrain.Transmission.PrimaryGearReduction</t>
+  </si>
+  <si>
+    <t>Powertrain.Transmission.FinalGearReduction</t>
+  </si>
+  <si>
+    <t>Powertrain.Transmission.GearRatio(1)</t>
+  </si>
+  <si>
+    <t>Powertrain.Transmission.GearRatio(2)</t>
+  </si>
+  <si>
+    <t>etc.</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Brakes.PedalRatio</t>
+  </si>
+  <si>
+    <t>Brakes.Calipers.PistonDiameter</t>
+  </si>
+  <si>
+    <t>Brakes.Calipers.PistonCount</t>
+  </si>
+  <si>
+    <t>Brakes.MasterCylinders.BoreDiameter</t>
+  </si>
+  <si>
+    <t>Brakes.Pad.CoefficientOfFriction</t>
+  </si>
+  <si>
+    <t>Brakes.Pad.Thickness</t>
+  </si>
+  <si>
+    <t>Brakes.Disc.OuterDiameter</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Inertia.MassBalance</t>
+  </si>
+  <si>
+    <t>tyremodel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -638,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -709,6 +835,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,11 +857,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B19" totalsRowShown="0">
-  <autoFilter ref="A1:B19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B19" totalsRowShown="0">
+  <autoFilter ref="A1:B19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Engine Speed [rpm]"/>
-    <tableColumn id="2" name="Torque [Nm]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Engine Speed [rpm]"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Torque [Nm]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -999,771 +1129,979 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.9453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="81.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="F1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="34"/>
       <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="15"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="33" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="2"/>
+      <c r="D4" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="9">
         <v>650</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="34"/>
       <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="2"/>
+      <c r="D5" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="13">
         <v>45</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="15"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="18">
         <v>3000</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="F6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="2"/>
+      <c r="D7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="18">
         <v>10</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="33" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="9">
+        <v>72</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="9">
         <v>-4.8</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="35"/>
       <c r="B9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="4">
+        <v>73</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="4">
         <v>-1.2</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="35"/>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="2"/>
+      <c r="D10" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="35"/>
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="2"/>
+      <c r="D11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="4">
         <v>1</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="21"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="35"/>
       <c r="B12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="4">
+        <v>71</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="4">
         <v>50</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="21"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="35"/>
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="2"/>
+      <c r="D13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="4">
         <v>1</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="21"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A14" s="34"/>
       <c r="B14" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="2"/>
+      <c r="D14" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="13">
         <v>1.2250000000000001</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="F14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="33" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="2"/>
+      <c r="D15" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="9">
         <v>250</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="35"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="2"/>
+      <c r="D16" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" s="4">
         <v>40</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="35"/>
       <c r="B17" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="4">
+        <v>77</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="4">
         <v>0.45</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="35"/>
       <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="2"/>
+      <c r="D18" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="4">
         <v>6</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="35"/>
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="2"/>
+      <c r="D19" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="4">
         <v>40</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="35"/>
       <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="2"/>
+      <c r="D20" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="4">
         <v>25</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A21" s="34"/>
       <c r="B21" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="2"/>
+      <c r="D21" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="13">
         <v>4</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="2"/>
+      <c r="D22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="9">
         <v>1</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="35"/>
       <c r="B23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="2"/>
+      <c r="D23" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="4">
         <v>330</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G23" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="35"/>
       <c r="B24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="2"/>
+      <c r="D24" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="4">
         <v>-1E-3</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="35"/>
       <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="2"/>
+      <c r="D25" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" s="4">
         <v>2</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="35"/>
       <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="2"/>
+      <c r="D26" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" s="4">
         <v>250</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G26" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="35"/>
       <c r="B27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="2"/>
+      <c r="D27" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="4">
         <v>1E-4</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G27" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="35"/>
       <c r="B28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="2"/>
+      <c r="D28" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" s="4">
         <v>2</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="35"/>
       <c r="B29" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="2"/>
+      <c r="D29" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29" s="4">
         <v>250</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G29" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="35"/>
       <c r="B30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="2"/>
+      <c r="D30" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E30" s="4">
         <v>1E-4</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G30" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="35"/>
       <c r="B31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="2"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4">
         <v>800</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A32" s="34"/>
       <c r="B32" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="13">
         <v>1000</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="F32" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G32" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="33" t="s">
         <v>50</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="2"/>
+      <c r="D33" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E33" s="9">
         <v>1</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E33" s="11"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="35"/>
       <c r="B34" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="2"/>
+      <c r="D34" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="4">
         <v>0.35</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A35" s="34"/>
       <c r="B35" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="2"/>
+      <c r="D35" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E35" s="22">
         <v>47200000</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="F35" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G35" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="11"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="2"/>
+      <c r="D36" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="31"/>
       <c r="B37" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="D37" s="7" t="s">
+      <c r="G37" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="E37" s="29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="31"/>
       <c r="B38" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="6">
+        <v>74</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="6">
         <v>1</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="31"/>
       <c r="B39" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="6">
+        <v>75</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E39" s="6">
         <v>0.92</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E39" s="29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="31"/>
       <c r="B40" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" s="6">
+        <v>76</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E40" s="6">
         <v>0.98</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G40" s="29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="31"/>
       <c r="B41" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="4">
+        <v>59</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E41" s="4">
         <v>1</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G41" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="31"/>
       <c r="B42" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="4">
+        <v>60</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E42" s="4">
         <v>7</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" s="21"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G42" s="21"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="31"/>
       <c r="B43" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" s="4">
+        <v>61</v>
+      </c>
+      <c r="C43" s="27"/>
+      <c r="D43" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E43" s="4">
         <v>2.57</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="21"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" s="21"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="31"/>
       <c r="B44" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44" s="4">
+        <v>62</v>
+      </c>
+      <c r="C44" s="27"/>
+      <c r="D44" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E44" s="4">
         <v>2.11</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E44" s="21"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G44" s="21"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="31"/>
       <c r="B45" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="4">
+        <v>63</v>
+      </c>
+      <c r="C45" s="27"/>
+      <c r="D45" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="4">
         <v>1.75</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E45" s="21"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" s="21"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="31"/>
       <c r="B46" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="4">
+        <v>64</v>
+      </c>
+      <c r="C46" s="27"/>
+      <c r="D46" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="4">
         <v>1.46</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E46" s="21"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G46" s="21"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="31"/>
       <c r="B47" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" s="4">
+        <v>65</v>
+      </c>
+      <c r="C47" s="27"/>
+      <c r="D47" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47" s="4">
         <v>1.29</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E47" s="21"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="21"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="31"/>
       <c r="B48" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" s="4">
+        <v>66</v>
+      </c>
+      <c r="C48" s="27"/>
+      <c r="D48" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E48" s="4">
         <v>1.1299999999999999</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E48" s="21"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G48" s="21"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="31"/>
       <c r="B49" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="C49" s="4">
+        <v>67</v>
+      </c>
+      <c r="C49" s="27"/>
+      <c r="D49" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="4">
         <v>1</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E49" s="21"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G49" s="21"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="31"/>
       <c r="B50" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C50" s="4"/>
+        <v>68</v>
+      </c>
+      <c r="C50" s="27"/>
       <c r="D50" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E50" s="21"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G50" s="21"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="31"/>
       <c r="B51" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C51" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="C51" s="27"/>
       <c r="D51" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E51" s="21"/>
-    </row>
-    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G51" s="21"/>
+    </row>
+    <row r="52" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A52" s="32"/>
       <c r="B52" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E52" s="15"/>
+        <v>70</v>
+      </c>
+      <c r="C52" s="27"/>
+      <c r="D52" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E52" s="13"/>
+      <c r="F52" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G52" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1781,20 +2119,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1802,7 +2140,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -1810,7 +2148,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
@@ -1818,7 +2156,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>3000</v>
       </c>
@@ -1826,7 +2164,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>4000</v>
       </c>
@@ -1834,7 +2172,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>5000</v>
       </c>
@@ -1842,7 +2180,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>6000</v>
       </c>
@@ -1850,7 +2188,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>7000</v>
       </c>
@@ -1858,7 +2196,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>8000</v>
       </c>
@@ -1866,7 +2204,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>9000</v>
       </c>
@@ -1874,7 +2212,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>10000</v>
       </c>
@@ -1882,7 +2220,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>11000</v>
       </c>
@@ -1890,7 +2228,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>12000</v>
       </c>
@@ -1898,7 +2236,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>13000</v>
       </c>
@@ -1906,7 +2244,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>14000</v>
       </c>
@@ -1914,7 +2252,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>15000</v>
       </c>
@@ -1922,7 +2260,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>16000</v>
       </c>
@@ -1930,7 +2268,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>17000</v>
       </c>
@@ -1938,7 +2276,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>18000</v>
       </c>

</xml_diff>

<commit_message>
Chnaged Excel sgeet to incorpertae more Accurate tire data
</commit_message>
<xml_diff>
--- a/Formula 1.xlsx
+++ b/Formula 1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Youtube VD\Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quinh\OneDrive\Documents\Open Lap Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91004D53-B71A-4239-BDA5-2EC1857EC7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8745" windowHeight="12405"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="102">
   <si>
     <t>General</t>
   </si>
@@ -328,12 +329,15 @@
   </si>
   <si>
     <t>From crancskaft to Input shaft.</t>
+  </si>
+  <si>
+    <t>jj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -727,11 +731,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B19" totalsRowShown="0">
-  <autoFilter ref="A1:B19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B19" totalsRowShown="0">
+  <autoFilter ref="A1:B19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Engine Speed [rpm]"/>
-    <tableColumn id="2" name="Torque [Nm]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Engine Speed [rpm]"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Torque [Nm]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -999,11 +1003,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,7 +1019,7 @@
     <col min="5" max="5" width="81.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>45</v>
       </c>
@@ -1032,7 +1036,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -1049,7 +1053,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34"/>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -1062,7 +1066,7 @@
       </c>
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>12</v>
       </c>
@@ -1077,7 +1081,7 @@
       </c>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34"/>
       <c r="B5" s="12" t="s">
         <v>4</v>
@@ -1090,7 +1094,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -1105,7 +1109,7 @@
       </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
@@ -1122,7 +1126,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>14</v>
       </c>
@@ -1139,7 +1143,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="35"/>
       <c r="B9" s="2" t="s">
         <v>74</v>
@@ -1154,7 +1158,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="35"/>
       <c r="B10" s="2" t="s">
         <v>21</v>
@@ -1167,7 +1171,7 @@
       </c>
       <c r="E10" s="21"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="35"/>
       <c r="B11" s="2" t="s">
         <v>22</v>
@@ -1179,8 +1183,11 @@
         <v>38</v>
       </c>
       <c r="E11" s="21"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
       <c r="B12" s="2" t="s">
         <v>72</v>
@@ -1193,7 +1200,7 @@
       </c>
       <c r="E12" s="21"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
       <c r="B13" s="2" t="s">
         <v>17</v>
@@ -1206,7 +1213,7 @@
       </c>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="34"/>
       <c r="B14" s="12" t="s">
         <v>23</v>
@@ -1221,7 +1228,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>20</v>
       </c>
@@ -1238,7 +1245,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="35"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
@@ -1781,7 +1788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>